<commit_message>
Update Solution to 2020
</commit_message>
<xml_diff>
--- a/RFLTools Command Reference.xlsx
+++ b/RFLTools Command Reference.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="324">
   <si>
     <t>RFL Tools Command Listing</t>
   </si>
@@ -990,6 +990,12 @@
   </si>
   <si>
     <t>Changes all the entities in a selected block to a desired colour</t>
+  </si>
+  <si>
+    <t>CHTRANS</t>
+  </si>
+  <si>
+    <t>Changes all the entities in a selected block to a desired transparency</t>
   </si>
 </sst>
 </file>
@@ -1358,10 +1364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B165"/>
+  <dimension ref="A1:B166"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1553,1121 +1559,1129 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="B26" t="s">
-        <v>311</v>
+        <v>323</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>310</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>311</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>292</v>
+        <v>49</v>
       </c>
       <c r="B32" t="s">
-        <v>293</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>292</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>293</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B36" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B37" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B38" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>288</v>
+        <v>61</v>
       </c>
       <c r="B39" t="s">
-        <v>289</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>288</v>
       </c>
       <c r="B40" t="s">
-        <v>64</v>
+        <v>289</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>306</v>
+        <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>307</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>306</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
+        <v>307</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B43" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B44" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="B45" t="s">
-        <v>186</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>71</v>
+        <v>185</v>
       </c>
       <c r="B46" t="s">
-        <v>72</v>
+        <v>186</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B47" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B48" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B49" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B50" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B51" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>296</v>
+        <v>81</v>
       </c>
       <c r="B52" t="s">
-        <v>297</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>83</v>
+        <v>296</v>
       </c>
       <c r="B53" t="s">
-        <v>84</v>
+        <v>297</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B54" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B55" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B56" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B57" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B58" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B59" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B60" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B61" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B62" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B63" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B64" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B65" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B66" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>318</v>
+        <v>109</v>
       </c>
       <c r="B67" t="s">
-        <v>319</v>
+        <v>110</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>111</v>
+        <v>318</v>
       </c>
       <c r="B68" t="s">
-        <v>112</v>
+        <v>319</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B69" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>298</v>
+        <v>113</v>
       </c>
       <c r="B70" t="s">
-        <v>299</v>
+        <v>114</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>115</v>
+        <v>298</v>
       </c>
       <c r="B71" t="s">
-        <v>116</v>
+        <v>299</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>312</v>
+        <v>115</v>
       </c>
       <c r="B72" t="s">
-        <v>313</v>
+        <v>116</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>290</v>
+        <v>312</v>
       </c>
       <c r="B73" t="s">
-        <v>291</v>
+        <v>313</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>179</v>
+        <v>290</v>
       </c>
       <c r="B74" t="s">
-        <v>180</v>
+        <v>291</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>117</v>
+        <v>179</v>
       </c>
       <c r="B75" t="s">
-        <v>118</v>
+        <v>180</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B76" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B77" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B78" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B79" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B80" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B81" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B82" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B83" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B84" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B85" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B86" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B87" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B88" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B89" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B90" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B91" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B92" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B93" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B94" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B95" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B96" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>300</v>
+        <v>157</v>
       </c>
       <c r="B97" t="s">
-        <v>301</v>
+        <v>158</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>159</v>
+        <v>300</v>
       </c>
       <c r="B98" t="s">
-        <v>160</v>
+        <v>301</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B99" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B100" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B101" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B102" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B103" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B104" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B105" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B106" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B107" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>294</v>
+        <v>177</v>
       </c>
       <c r="B108" t="s">
-        <v>295</v>
+        <v>178</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>187</v>
+        <v>294</v>
       </c>
       <c r="B109" t="s">
-        <v>188</v>
+        <v>295</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B110" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>314</v>
+        <v>189</v>
       </c>
       <c r="B111" t="s">
-        <v>315</v>
+        <v>190</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>191</v>
+        <v>314</v>
       </c>
       <c r="B112" t="s">
-        <v>192</v>
+        <v>315</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B113" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B114" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B115" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B116" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B117" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B118" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B119" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B120" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B121" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B122" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B123" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B124" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>183</v>
+        <v>215</v>
       </c>
       <c r="B125" t="s">
-        <v>184</v>
+        <v>216</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>217</v>
+        <v>183</v>
       </c>
       <c r="B126" t="s">
-        <v>218</v>
+        <v>184</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B127" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B128" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B129" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B130" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B131" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B132" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B133" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>302</v>
+        <v>231</v>
       </c>
       <c r="B134" t="s">
-        <v>303</v>
+        <v>232</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>233</v>
+        <v>302</v>
       </c>
       <c r="B135" t="s">
-        <v>234</v>
+        <v>303</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>316</v>
+        <v>233</v>
       </c>
       <c r="B136" t="s">
-        <v>317</v>
+        <v>234</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>235</v>
+        <v>316</v>
       </c>
       <c r="B137" t="s">
-        <v>236</v>
+        <v>317</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B138" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B139" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B140" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B141" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B142" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>181</v>
+        <v>245</v>
       </c>
       <c r="B143" t="s">
-        <v>182</v>
+        <v>246</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>247</v>
+        <v>181</v>
       </c>
       <c r="B144" t="s">
-        <v>248</v>
+        <v>182</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B145" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B146" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B147" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B148" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B149" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B150" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B151" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B152" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B153" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B154" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B155" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B156" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B157" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B158" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B159" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B160" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B161" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B162" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B163" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B164" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
+        <v>286</v>
+      </c>
+      <c r="B165" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>308</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B166" t="s">
         <v>309</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor revisions to QLSection
</commit_message>
<xml_diff>
--- a/RFLTools Command Reference.xlsx
+++ b/RFLTools Command Reference.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Lisp\GitHub\RFLTools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\CAVAN400HYP01\Reference\NTL\2. Common Library\2.5 CAD\2.5.4 Autodesk\Custom Programs\RFLTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E44E5D-64BC-4CF1-A129-4628AAB68FC9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEE92E8-70DF-4B70-819F-933B31C84B5C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="405" windowWidth="20145" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50040" yWindow="-2655" windowWidth="20145" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1005,9 +1005,6 @@
     <t>Tool to add custom vehicle to QuickTurn</t>
   </si>
   <si>
-    <t>QLSECTIONDB</t>
-  </si>
-  <si>
     <t>CREATELIDARDB</t>
   </si>
   <si>
@@ -1021,6 +1018,9 @@
   </si>
   <si>
     <t>Draws a cros section from a Lidar point database (Note:  requires code found here http://www.theswamp.org/index.php?topic=28286.0)</t>
+  </si>
+  <si>
+    <t>QLSECTION</t>
   </si>
 </sst>
 </file>
@@ -1392,7 +1392,7 @@
   <dimension ref="A1:B170"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+      <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1472,10 +1472,10 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>328</v>
+      </c>
+      <c r="B12" t="s">
         <v>329</v>
-      </c>
-      <c r="B12" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1608,10 +1608,10 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>326</v>
+      </c>
+      <c r="B29" t="s">
         <v>327</v>
-      </c>
-      <c r="B29" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2144,10 +2144,10 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="B96" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
New Command - QuickProf
Utility for modelling a vehicle alone a 2D profile
</commit_message>
<xml_diff>
--- a/RFLTools Command Reference.xlsx
+++ b/RFLTools Command Reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Lisp\GitHub\RFLTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31D0469-F358-4194-A9A3-13ABAC5B506E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5686E233-E1DC-40F4-826B-5ED18588811D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50040" yWindow="-2655" windowWidth="20145" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-12720" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="336">
   <si>
     <t>RFL Tools Command Listing</t>
   </si>
@@ -1017,9 +1017,6 @@
     <t>Adds to a SQLITE Database using points found in a repo pts file</t>
   </si>
   <si>
-    <t>Draws a cros section from a Lidar point database (Note:  requires code found here http://www.theswamp.org/index.php?topic=28286.0)</t>
-  </si>
-  <si>
     <t>QLSECTION</t>
   </si>
   <si>
@@ -1027,6 +1024,15 @@
   </si>
   <si>
     <t>A utility to draw best fit lines within QLSection point section blocks</t>
+  </si>
+  <si>
+    <t>QLSECTIONPP</t>
+  </si>
+  <si>
+    <t>Draws a cross section from a Lidar point database (Note:  requires RFLTools DLL)</t>
+  </si>
+  <si>
+    <t>Draws a point to point section from a Lidar point database (Note:  requires RFLTools DLL)</t>
   </si>
 </sst>
 </file>
@@ -1395,10 +1401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B171"/>
+  <dimension ref="A1:B172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1550,10 +1556,10 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>331</v>
+      </c>
+      <c r="B21" t="s">
         <v>332</v>
-      </c>
-      <c r="B21" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2158,601 +2164,609 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B97" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>151</v>
+        <v>333</v>
       </c>
       <c r="B98" t="s">
-        <v>152</v>
+        <v>335</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B99" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B100" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B101" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>300</v>
+        <v>157</v>
       </c>
       <c r="B102" t="s">
-        <v>301</v>
+        <v>158</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>324</v>
+        <v>300</v>
       </c>
       <c r="B103" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>159</v>
+        <v>324</v>
       </c>
       <c r="B104" t="s">
-        <v>160</v>
+        <v>325</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B105" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B106" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B107" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B108" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B109" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B110" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B111" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B112" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B113" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>294</v>
+        <v>177</v>
       </c>
       <c r="B114" t="s">
-        <v>295</v>
+        <v>178</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>187</v>
+        <v>294</v>
       </c>
       <c r="B115" t="s">
-        <v>188</v>
+        <v>295</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B116" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>314</v>
+        <v>189</v>
       </c>
       <c r="B117" t="s">
-        <v>315</v>
+        <v>190</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>191</v>
+        <v>314</v>
       </c>
       <c r="B118" t="s">
-        <v>192</v>
+        <v>315</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B119" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B120" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B121" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B122" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B123" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B124" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B125" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B126" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B127" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B128" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B129" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B130" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>183</v>
+        <v>215</v>
       </c>
       <c r="B131" t="s">
-        <v>184</v>
+        <v>216</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>217</v>
+        <v>183</v>
       </c>
       <c r="B132" t="s">
-        <v>218</v>
+        <v>184</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B133" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B134" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B135" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B136" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B137" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B138" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B139" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>302</v>
+        <v>231</v>
       </c>
       <c r="B140" t="s">
-        <v>303</v>
+        <v>232</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>233</v>
+        <v>302</v>
       </c>
       <c r="B141" t="s">
-        <v>234</v>
+        <v>303</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>316</v>
+        <v>233</v>
       </c>
       <c r="B142" t="s">
-        <v>317</v>
+        <v>234</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>235</v>
+        <v>316</v>
       </c>
       <c r="B143" t="s">
-        <v>236</v>
+        <v>317</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B144" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B145" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B146" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B147" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B148" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>181</v>
+        <v>245</v>
       </c>
       <c r="B149" t="s">
-        <v>182</v>
+        <v>246</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>247</v>
+        <v>181</v>
       </c>
       <c r="B150" t="s">
-        <v>248</v>
+        <v>182</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B151" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B152" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B153" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B154" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B155" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B156" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B157" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B158" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B159" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B160" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B161" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B162" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B163" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B164" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B165" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B166" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B167" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B168" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B169" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B170" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
+        <v>286</v>
+      </c>
+      <c r="B171" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
         <v>308</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B172" t="s">
         <v>309</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new command to reference file
</commit_message>
<xml_diff>
--- a/RFLTools Command Reference.xlsx
+++ b/RFLTools Command Reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Lisp\GitHub\RFLTools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\LISP\GitHub\RFLTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF324A91-659D-4DBC-8E34-2DC17E55BF69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBCBE3A-7509-4BA6-A8EA-450B12DC28AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42435" yWindow="-795" windowWidth="21945" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="43200" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="354">
   <si>
     <t>RFL Tools Command Listing</t>
   </si>
@@ -1081,6 +1081,12 @@
   </si>
   <si>
     <t>Converts the current RFL Profile from Ground to Grid (work in progress, must be scaled at 0,0)</t>
+  </si>
+  <si>
+    <t>RALIGNXML</t>
+  </si>
+  <si>
+    <t>Reads the alignment from a Land XML file</t>
   </si>
 </sst>
 </file>
@@ -1449,10 +1455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B180"/>
+  <dimension ref="A1:B181"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+      <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2396,489 +2402,497 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>174</v>
+        <v>352</v>
       </c>
       <c r="B120" t="s">
-        <v>175</v>
+        <v>353</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B121" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>291</v>
+        <v>176</v>
       </c>
       <c r="B122" t="s">
-        <v>292</v>
+        <v>177</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>186</v>
+        <v>291</v>
       </c>
       <c r="B123" t="s">
-        <v>187</v>
+        <v>292</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B124" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>311</v>
+        <v>188</v>
       </c>
       <c r="B125" t="s">
-        <v>312</v>
+        <v>189</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>190</v>
+        <v>311</v>
       </c>
       <c r="B126" t="s">
-        <v>191</v>
+        <v>312</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B127" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B128" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B129" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>335</v>
+        <v>196</v>
       </c>
       <c r="B130" t="s">
-        <v>336</v>
+        <v>197</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>198</v>
+        <v>335</v>
       </c>
       <c r="B131" t="s">
-        <v>199</v>
+        <v>336</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B132" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B133" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B134" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B135" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B136" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B137" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B138" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>182</v>
+        <v>212</v>
       </c>
       <c r="B139" t="s">
-        <v>183</v>
+        <v>213</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
       <c r="B140" t="s">
-        <v>215</v>
+        <v>183</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B141" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B142" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B143" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B144" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B145" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>338</v>
+        <v>224</v>
       </c>
       <c r="B146" t="s">
-        <v>339</v>
+        <v>225</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>226</v>
+        <v>338</v>
       </c>
       <c r="B147" t="s">
-        <v>227</v>
+        <v>339</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B148" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>299</v>
+        <v>228</v>
       </c>
       <c r="B149" t="s">
-        <v>300</v>
+        <v>229</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>230</v>
+        <v>299</v>
       </c>
       <c r="B150" t="s">
-        <v>231</v>
+        <v>300</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>313</v>
+        <v>230</v>
       </c>
       <c r="B151" t="s">
-        <v>314</v>
+        <v>231</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>232</v>
+        <v>313</v>
       </c>
       <c r="B152" t="s">
-        <v>233</v>
+        <v>314</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B153" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B154" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B155" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B156" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B157" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>180</v>
+        <v>242</v>
       </c>
       <c r="B158" t="s">
-        <v>181</v>
+        <v>243</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>244</v>
+        <v>180</v>
       </c>
       <c r="B159" t="s">
-        <v>245</v>
+        <v>181</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B160" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B161" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B162" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B163" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B164" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B165" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B166" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B167" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B168" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B169" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B170" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B171" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B172" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B173" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B174" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B175" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B176" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B177" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B178" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B179" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
+        <v>283</v>
+      </c>
+      <c r="B180" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
         <v>305</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B181" t="s">
         <v>306</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update RFLTools Command Reference.xlsx
</commit_message>
<xml_diff>
--- a/RFLTools Command Reference.xlsx
+++ b/RFLTools Command Reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\LISP\GitHub\RFLTools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RLivingston\Documents\RFLTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBCBE3A-7509-4BA6-A8EA-450B12DC28AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA31FF2-0323-490A-B41D-413830346677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="43200" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="66345" yWindow="-9435" windowWidth="16050" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="356">
   <si>
     <t>RFL Tools Command Listing</t>
   </si>
@@ -1087,6 +1087,12 @@
   </si>
   <si>
     <t>Reads the alignment from a Land XML file</t>
+  </si>
+  <si>
+    <t>SCOPY</t>
+  </si>
+  <si>
+    <t>Extracts a C3D ground section line to a polyline</t>
   </si>
 </sst>
 </file>
@@ -1455,10 +1461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B181"/>
+  <dimension ref="A1:B182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B121" sqref="B121"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="B140" sqref="B140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2554,345 +2560,353 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>212</v>
+        <v>354</v>
       </c>
       <c r="B139" t="s">
-        <v>213</v>
+        <v>355</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>182</v>
+        <v>212</v>
       </c>
       <c r="B140" t="s">
-        <v>183</v>
+        <v>213</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
       <c r="B141" t="s">
-        <v>215</v>
+        <v>183</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B142" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B143" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B144" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B145" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B146" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>338</v>
+        <v>224</v>
       </c>
       <c r="B147" t="s">
-        <v>339</v>
+        <v>225</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>226</v>
+        <v>338</v>
       </c>
       <c r="B148" t="s">
-        <v>227</v>
+        <v>339</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B149" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>299</v>
+        <v>228</v>
       </c>
       <c r="B150" t="s">
-        <v>300</v>
+        <v>229</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>230</v>
+        <v>299</v>
       </c>
       <c r="B151" t="s">
-        <v>231</v>
+        <v>300</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>313</v>
+        <v>230</v>
       </c>
       <c r="B152" t="s">
-        <v>314</v>
+        <v>231</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>232</v>
+        <v>313</v>
       </c>
       <c r="B153" t="s">
-        <v>233</v>
+        <v>314</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B154" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B155" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B156" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B157" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B158" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>180</v>
+        <v>242</v>
       </c>
       <c r="B159" t="s">
-        <v>181</v>
+        <v>243</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>244</v>
+        <v>180</v>
       </c>
       <c r="B160" t="s">
-        <v>245</v>
+        <v>181</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B161" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B162" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B163" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B164" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B165" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B166" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B167" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B168" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B169" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B170" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B171" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B172" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B173" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B174" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B175" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B176" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B177" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B178" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B179" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B180" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
+        <v>283</v>
+      </c>
+      <c r="B181" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
         <v>305</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B182" t="s">
         <v>306</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New command - Rotate2PL
</commit_message>
<xml_diff>
--- a/RFLTools Command Reference.xlsx
+++ b/RFLTools Command Reference.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RLivingston\Documents\RFLTools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\LISP\GitHub\RFLTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA31FF2-0323-490A-B41D-413830346677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE3862B-21AE-48C8-8B02-57199C4385B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="66345" yWindow="-9435" windowWidth="16050" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="43200" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="358">
   <si>
     <t>RFL Tools Command Listing</t>
   </si>
@@ -1093,6 +1093,12 @@
   </si>
   <si>
     <t>Extracts a C3D ground section line to a polyline</t>
+  </si>
+  <si>
+    <t>ROTATE2PL</t>
+  </si>
+  <si>
+    <t>Rotates blocks to be aligned with selected polylines</t>
   </si>
 </sst>
 </file>
@@ -1461,10 +1467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B182"/>
+  <dimension ref="A1:B183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="B140" sqref="B140"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2464,449 +2470,457 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>190</v>
+        <v>356</v>
       </c>
       <c r="B127" t="s">
-        <v>191</v>
+        <v>357</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B128" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B129" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B130" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>335</v>
+        <v>196</v>
       </c>
       <c r="B131" t="s">
-        <v>336</v>
+        <v>197</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>198</v>
+        <v>335</v>
       </c>
       <c r="B132" t="s">
-        <v>199</v>
+        <v>336</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B133" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B134" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B135" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B136" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B137" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B138" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>354</v>
+        <v>210</v>
       </c>
       <c r="B139" t="s">
-        <v>355</v>
+        <v>211</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>212</v>
+        <v>354</v>
       </c>
       <c r="B140" t="s">
-        <v>213</v>
+        <v>355</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>182</v>
+        <v>212</v>
       </c>
       <c r="B141" t="s">
-        <v>183</v>
+        <v>213</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
       <c r="B142" t="s">
-        <v>215</v>
+        <v>183</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B143" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B144" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B145" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B146" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B147" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>338</v>
+        <v>224</v>
       </c>
       <c r="B148" t="s">
-        <v>339</v>
+        <v>225</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>226</v>
+        <v>338</v>
       </c>
       <c r="B149" t="s">
-        <v>227</v>
+        <v>339</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B150" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>299</v>
+        <v>228</v>
       </c>
       <c r="B151" t="s">
-        <v>300</v>
+        <v>229</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>230</v>
+        <v>299</v>
       </c>
       <c r="B152" t="s">
-        <v>231</v>
+        <v>300</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>313</v>
+        <v>230</v>
       </c>
       <c r="B153" t="s">
-        <v>314</v>
+        <v>231</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>232</v>
+        <v>313</v>
       </c>
       <c r="B154" t="s">
-        <v>233</v>
+        <v>314</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B155" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B156" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B157" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B158" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B159" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>180</v>
+        <v>242</v>
       </c>
       <c r="B160" t="s">
-        <v>181</v>
+        <v>243</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>244</v>
+        <v>180</v>
       </c>
       <c r="B161" t="s">
-        <v>245</v>
+        <v>181</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B162" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B163" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B164" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B165" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B166" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B167" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B168" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B169" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B170" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B171" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B172" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B173" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B174" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B175" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B176" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B177" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B178" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B179" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B180" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B181" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
+        <v>283</v>
+      </c>
+      <c r="B182" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
         <v>305</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B183" t="s">
         <v>306</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Neew commands GETZ2, Z2N and Z2P
Utility for finding nested blocks
</commit_message>
<xml_diff>
--- a/RFLTools Command Reference.xlsx
+++ b/RFLTools Command Reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\LISP\GitHub\RFLTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE3862B-21AE-48C8-8B02-57199C4385B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C5B21B-3705-4026-84C8-897CBB1DFA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="43200" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15300" yWindow="3585" windowWidth="43200" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="364">
   <si>
     <t>RFL Tools Command Listing</t>
   </si>
@@ -1099,6 +1099,24 @@
   </si>
   <si>
     <t>Rotates blocks to be aligned with selected polylines</t>
+  </si>
+  <si>
+    <t>GETZ2</t>
+  </si>
+  <si>
+    <t>Searches a block or xref for nested blocks (useful for finding all blocks such as signs).  Used with Z2N and Z2P</t>
+  </si>
+  <si>
+    <t>Z2N</t>
+  </si>
+  <si>
+    <t>Zooms to the next block found with GETZ2</t>
+  </si>
+  <si>
+    <t>Z2P</t>
+  </si>
+  <si>
+    <t>Zooms to the previous block found with GETZ2</t>
   </si>
 </sst>
 </file>
@@ -1467,10 +1485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B183"/>
+  <dimension ref="A1:B186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="B128" sqref="B128"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="B187" sqref="B187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,994 +1952,1018 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>83</v>
+        <v>358</v>
       </c>
       <c r="B60" t="s">
-        <v>84</v>
+        <v>359</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B61" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B62" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B63" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B64" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B65" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B66" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B67" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B68" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B69" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B70" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B71" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B72" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B73" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>315</v>
+        <v>109</v>
       </c>
       <c r="B74" t="s">
-        <v>316</v>
+        <v>110</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>111</v>
+        <v>315</v>
       </c>
       <c r="B75" t="s">
-        <v>112</v>
+        <v>316</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B76" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>295</v>
+        <v>113</v>
       </c>
       <c r="B77" t="s">
-        <v>296</v>
+        <v>114</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>115</v>
+        <v>295</v>
       </c>
       <c r="B78" t="s">
-        <v>116</v>
+        <v>296</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>309</v>
+        <v>115</v>
       </c>
       <c r="B79" t="s">
-        <v>310</v>
+        <v>116</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>287</v>
+        <v>309</v>
       </c>
       <c r="B80" t="s">
-        <v>288</v>
+        <v>310</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>178</v>
+        <v>287</v>
       </c>
       <c r="B81" t="s">
-        <v>179</v>
+        <v>288</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>117</v>
+        <v>178</v>
       </c>
       <c r="B82" t="s">
-        <v>118</v>
+        <v>179</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B83" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B84" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B85" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B86" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B87" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B88" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B89" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B90" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B91" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B92" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B93" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B94" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B95" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B96" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B97" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B98" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>348</v>
+        <v>147</v>
       </c>
       <c r="B99" t="s">
-        <v>350</v>
+        <v>148</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B100" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>149</v>
+        <v>349</v>
       </c>
       <c r="B101" t="s">
-        <v>150</v>
+        <v>351</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>327</v>
+        <v>149</v>
       </c>
       <c r="B102" t="s">
-        <v>331</v>
+        <v>150</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B103" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>151</v>
+        <v>330</v>
       </c>
       <c r="B104" t="s">
-        <v>152</v>
+        <v>332</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B105" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B106" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>333</v>
+        <v>155</v>
       </c>
       <c r="B107" t="s">
-        <v>334</v>
+        <v>156</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>157</v>
+        <v>333</v>
       </c>
       <c r="B108" t="s">
-        <v>158</v>
+        <v>334</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>297</v>
+        <v>157</v>
       </c>
       <c r="B109" t="s">
-        <v>298</v>
+        <v>158</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
       <c r="B110" t="s">
-        <v>322</v>
+        <v>298</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>340</v>
+        <v>321</v>
       </c>
       <c r="B111" t="s">
-        <v>341</v>
+        <v>322</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>159</v>
+        <v>340</v>
       </c>
       <c r="B112" t="s">
-        <v>160</v>
+        <v>341</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B113" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B114" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B115" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B116" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B117" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B118" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B119" t="s">
-        <v>337</v>
+        <v>172</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>352</v>
+        <v>173</v>
       </c>
       <c r="B120" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>174</v>
+        <v>352</v>
       </c>
       <c r="B121" t="s">
-        <v>175</v>
+        <v>353</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B122" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>291</v>
+        <v>176</v>
       </c>
       <c r="B123" t="s">
-        <v>292</v>
+        <v>177</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>186</v>
+        <v>291</v>
       </c>
       <c r="B124" t="s">
-        <v>187</v>
+        <v>292</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B125" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>311</v>
+        <v>188</v>
       </c>
       <c r="B126" t="s">
-        <v>312</v>
+        <v>189</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>356</v>
+        <v>311</v>
       </c>
       <c r="B127" t="s">
-        <v>357</v>
+        <v>312</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>190</v>
+        <v>356</v>
       </c>
       <c r="B128" t="s">
-        <v>191</v>
+        <v>357</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B129" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B130" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B131" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>335</v>
+        <v>196</v>
       </c>
       <c r="B132" t="s">
-        <v>336</v>
+        <v>197</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>198</v>
+        <v>335</v>
       </c>
       <c r="B133" t="s">
-        <v>199</v>
+        <v>336</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B134" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B135" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B136" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B137" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B138" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B139" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>354</v>
+        <v>210</v>
       </c>
       <c r="B140" t="s">
-        <v>355</v>
+        <v>211</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>212</v>
+        <v>354</v>
       </c>
       <c r="B141" t="s">
-        <v>213</v>
+        <v>355</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>182</v>
+        <v>212</v>
       </c>
       <c r="B142" t="s">
-        <v>183</v>
+        <v>213</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
       <c r="B143" t="s">
-        <v>215</v>
+        <v>183</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B144" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B145" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B146" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B147" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B148" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>338</v>
+        <v>224</v>
       </c>
       <c r="B149" t="s">
-        <v>339</v>
+        <v>225</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>226</v>
+        <v>338</v>
       </c>
       <c r="B150" t="s">
-        <v>227</v>
+        <v>339</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B151" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>299</v>
+        <v>228</v>
       </c>
       <c r="B152" t="s">
-        <v>300</v>
+        <v>229</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>230</v>
+        <v>299</v>
       </c>
       <c r="B153" t="s">
-        <v>231</v>
+        <v>300</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>313</v>
+        <v>230</v>
       </c>
       <c r="B154" t="s">
-        <v>314</v>
+        <v>231</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>232</v>
+        <v>313</v>
       </c>
       <c r="B155" t="s">
-        <v>233</v>
+        <v>314</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B156" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B157" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B158" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B159" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B160" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>180</v>
+        <v>242</v>
       </c>
       <c r="B161" t="s">
-        <v>181</v>
+        <v>243</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>244</v>
+        <v>180</v>
       </c>
       <c r="B162" t="s">
-        <v>245</v>
+        <v>181</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B163" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B164" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B165" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B166" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B167" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B168" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B169" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B170" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B171" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B172" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B173" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B174" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B175" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B176" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B177" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B178" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B179" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B180" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B181" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B182" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
+        <v>283</v>
+      </c>
+      <c r="B183" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
         <v>305</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B184" t="s">
         <v>306</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>360</v>
+      </c>
+      <c r="B185" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>362</v>
+      </c>
+      <c r="B186" t="s">
+        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added DXLINE to list
</commit_message>
<xml_diff>
--- a/RFLTools Command Reference.xlsx
+++ b/RFLTools Command Reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\LISP\GitHub\RFLTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44B1BDA-693C-492F-B0B8-3B745D263228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F351E78-C707-4B66-86C8-6F14D4EAD030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32670" yWindow="7305" windowWidth="23820" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6435" yWindow="7185" windowWidth="43200" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="368">
   <si>
     <t>RFL Tools Command Listing</t>
   </si>
@@ -1123,6 +1123,12 @@
   </si>
   <si>
     <t>A utility for importing LKI Placemarks from a BCMoTI KML file</t>
+  </si>
+  <si>
+    <t>DXLINE</t>
+  </si>
+  <si>
+    <t>Draws an XLINE at a given or selected station</t>
   </si>
 </sst>
 </file>
@@ -1491,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B187"/>
+  <dimension ref="A1:B188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1886,1097 +1892,1105 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>69</v>
+        <v>366</v>
       </c>
       <c r="B51" t="s">
-        <v>70</v>
+        <v>367</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>184</v>
+        <v>69</v>
       </c>
       <c r="B52" t="s">
-        <v>185</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>71</v>
+        <v>184</v>
       </c>
       <c r="B53" t="s">
-        <v>72</v>
+        <v>185</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B54" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B55" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B56" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B57" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B58" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>293</v>
+        <v>81</v>
       </c>
       <c r="B59" t="s">
-        <v>294</v>
+        <v>82</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>358</v>
+        <v>293</v>
       </c>
       <c r="B60" t="s">
-        <v>359</v>
+        <v>294</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>83</v>
+        <v>358</v>
       </c>
       <c r="B61" t="s">
-        <v>84</v>
+        <v>359</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B62" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B63" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B64" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B65" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B66" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B67" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B68" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>364</v>
+        <v>97</v>
       </c>
       <c r="B69" t="s">
-        <v>365</v>
+        <v>98</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>99</v>
+        <v>364</v>
       </c>
       <c r="B70" t="s">
-        <v>100</v>
+        <v>365</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B71" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B72" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B73" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B74" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B75" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>315</v>
+        <v>109</v>
       </c>
       <c r="B76" t="s">
-        <v>316</v>
+        <v>110</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>111</v>
+        <v>315</v>
       </c>
       <c r="B77" t="s">
-        <v>112</v>
+        <v>316</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B78" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>295</v>
+        <v>113</v>
       </c>
       <c r="B79" t="s">
-        <v>296</v>
+        <v>114</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>115</v>
+        <v>295</v>
       </c>
       <c r="B80" t="s">
-        <v>116</v>
+        <v>296</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>309</v>
+        <v>115</v>
       </c>
       <c r="B81" t="s">
-        <v>310</v>
+        <v>116</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>287</v>
+        <v>309</v>
       </c>
       <c r="B82" t="s">
-        <v>288</v>
+        <v>310</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>178</v>
+        <v>287</v>
       </c>
       <c r="B83" t="s">
-        <v>179</v>
+        <v>288</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>117</v>
+        <v>178</v>
       </c>
       <c r="B84" t="s">
-        <v>118</v>
+        <v>179</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B85" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B86" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B87" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B88" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B89" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B90" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B91" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B92" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B93" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B94" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B95" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B96" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B97" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B98" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B99" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B100" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>348</v>
+        <v>147</v>
       </c>
       <c r="B101" t="s">
-        <v>350</v>
+        <v>148</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B102" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>149</v>
+        <v>349</v>
       </c>
       <c r="B103" t="s">
-        <v>150</v>
+        <v>351</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>327</v>
+        <v>149</v>
       </c>
       <c r="B104" t="s">
-        <v>331</v>
+        <v>150</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B105" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>151</v>
+        <v>330</v>
       </c>
       <c r="B106" t="s">
-        <v>152</v>
+        <v>332</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B107" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B108" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>333</v>
+        <v>155</v>
       </c>
       <c r="B109" t="s">
-        <v>334</v>
+        <v>156</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>157</v>
+        <v>333</v>
       </c>
       <c r="B110" t="s">
-        <v>158</v>
+        <v>334</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>297</v>
+        <v>157</v>
       </c>
       <c r="B111" t="s">
-        <v>298</v>
+        <v>158</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
       <c r="B112" t="s">
-        <v>322</v>
+        <v>298</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>340</v>
+        <v>321</v>
       </c>
       <c r="B113" t="s">
-        <v>341</v>
+        <v>322</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>159</v>
+        <v>340</v>
       </c>
       <c r="B114" t="s">
-        <v>160</v>
+        <v>341</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B115" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B116" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B117" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B118" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B119" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B120" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B121" t="s">
-        <v>337</v>
+        <v>172</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>352</v>
+        <v>173</v>
       </c>
       <c r="B122" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>174</v>
+        <v>352</v>
       </c>
       <c r="B123" t="s">
-        <v>175</v>
+        <v>353</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B124" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>291</v>
+        <v>176</v>
       </c>
       <c r="B125" t="s">
-        <v>292</v>
+        <v>177</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>186</v>
+        <v>291</v>
       </c>
       <c r="B126" t="s">
-        <v>187</v>
+        <v>292</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B127" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>311</v>
+        <v>188</v>
       </c>
       <c r="B128" t="s">
-        <v>312</v>
+        <v>189</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>356</v>
+        <v>311</v>
       </c>
       <c r="B129" t="s">
-        <v>357</v>
+        <v>312</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>190</v>
+        <v>356</v>
       </c>
       <c r="B130" t="s">
-        <v>191</v>
+        <v>357</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B131" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B132" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B133" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>335</v>
+        <v>196</v>
       </c>
       <c r="B134" t="s">
-        <v>336</v>
+        <v>197</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>198</v>
+        <v>335</v>
       </c>
       <c r="B135" t="s">
-        <v>199</v>
+        <v>336</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B136" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B137" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B138" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B139" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B140" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B141" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>354</v>
+        <v>210</v>
       </c>
       <c r="B142" t="s">
-        <v>355</v>
+        <v>211</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>212</v>
+        <v>354</v>
       </c>
       <c r="B143" t="s">
-        <v>213</v>
+        <v>355</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>182</v>
+        <v>212</v>
       </c>
       <c r="B144" t="s">
-        <v>183</v>
+        <v>213</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
       <c r="B145" t="s">
-        <v>215</v>
+        <v>183</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B146" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B147" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B148" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B149" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B150" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>338</v>
+        <v>224</v>
       </c>
       <c r="B151" t="s">
-        <v>339</v>
+        <v>225</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>226</v>
+        <v>338</v>
       </c>
       <c r="B152" t="s">
-        <v>227</v>
+        <v>339</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B153" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>299</v>
+        <v>228</v>
       </c>
       <c r="B154" t="s">
-        <v>300</v>
+        <v>229</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>230</v>
+        <v>299</v>
       </c>
       <c r="B155" t="s">
-        <v>231</v>
+        <v>300</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>313</v>
+        <v>230</v>
       </c>
       <c r="B156" t="s">
-        <v>314</v>
+        <v>231</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>232</v>
+        <v>313</v>
       </c>
       <c r="B157" t="s">
-        <v>233</v>
+        <v>314</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B158" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B159" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B160" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B161" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B162" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>180</v>
+        <v>242</v>
       </c>
       <c r="B163" t="s">
-        <v>181</v>
+        <v>243</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>244</v>
+        <v>180</v>
       </c>
       <c r="B164" t="s">
-        <v>245</v>
+        <v>181</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B165" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B166" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B167" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B168" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B169" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B170" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B171" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B172" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B173" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B174" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B175" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B176" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B177" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B178" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B179" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B180" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B181" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B182" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B183" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B184" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>305</v>
+        <v>283</v>
       </c>
       <c r="B185" t="s">
-        <v>306</v>
+        <v>284</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>360</v>
+        <v>305</v>
       </c>
       <c r="B186" t="s">
-        <v>361</v>
+        <v>306</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
+        <v>360</v>
+      </c>
+      <c r="B187" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
         <v>362</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B188" t="s">
         <v>363</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Excel to include TXT2PLine
</commit_message>
<xml_diff>
--- a/RFLTools Command Reference.xlsx
+++ b/RFLTools Command Reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\LISP\GitHub\RFLTools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RLivingston\Documents\RFLTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216FD878-B858-45CD-8F83-100F3DD8AB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCDB2E4-0B1C-41F5-8E6C-BF96D07FB072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18315" yWindow="7005" windowWidth="27285" windowHeight="18375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30495" yWindow="-10815" windowWidth="30915" windowHeight="20775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="686">
   <si>
     <t>RFL Tools Command Listing</t>
   </si>
@@ -2077,6 +2077,12 @@
   </si>
   <si>
     <t>RFL:MAKEPLINE</t>
+  </si>
+  <si>
+    <t>TXT2PLINE</t>
+  </si>
+  <si>
+    <t>A utility to explode TEXT and MTEXT to polylines</t>
   </si>
 </sst>
 </file>
@@ -2445,10 +2451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B514"/>
+  <dimension ref="A1:B515"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
-      <selection activeCell="B308" sqref="B308"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="B164" sqref="B164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3736,1804 +3742,1812 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>238</v>
+        <v>684</v>
       </c>
       <c r="B163" t="s">
-        <v>239</v>
+        <v>685</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B164" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B165" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>180</v>
+        <v>242</v>
       </c>
       <c r="B166" t="s">
-        <v>181</v>
+        <v>243</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>370</v>
+        <v>180</v>
       </c>
       <c r="B167" t="s">
-        <v>371</v>
+        <v>181</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B168" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>244</v>
+        <v>368</v>
       </c>
       <c r="B169" t="s">
-        <v>245</v>
+        <v>369</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B170" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B171" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B172" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B173" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B174" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B175" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B176" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B177" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B178" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B179" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B180" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B181" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B182" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B183" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B184" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B185" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B186" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B187" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B188" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B189" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>305</v>
+        <v>283</v>
       </c>
       <c r="B190" t="s">
-        <v>306</v>
+        <v>284</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>360</v>
+        <v>305</v>
       </c>
       <c r="B191" t="s">
-        <v>361</v>
+        <v>306</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
+        <v>360</v>
+      </c>
+      <c r="B192" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
         <v>362</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B193" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A196" s="1" t="s">
+    <row r="197" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A197" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="B196" s="1" t="s">
+      <c r="B197" s="1" t="s">
         <v>393</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>490</v>
+        <v>390</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>374</v>
+        <v>490</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>673</v>
+        <v>374</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>391</v>
+        <v>673</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>472</v>
+        <v>391</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>375</v>
+        <v>472</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>392</v>
+        <v>375</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>376</v>
+        <v>392</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>394</v>
+        <v>376</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>541</v>
+        <v>394</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>487</v>
+        <v>544</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>377</v>
+        <v>487</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>510</v>
+        <v>377</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>378</v>
+        <v>511</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>539</v>
+        <v>378</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>379</v>
+        <v>540</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>554</v>
+        <v>379</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>380</v>
+        <v>554</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>538</v>
+        <v>399</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>444</v>
+        <v>538</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>417</v>
+        <v>445</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>521</v>
+        <v>417</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>462</v>
+        <v>521</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>446</v>
+        <v>462</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>545</v>
+        <v>446</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>400</v>
+        <v>545</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>381</v>
+        <v>400</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>522</v>
+        <v>381</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>418</v>
+        <v>524</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>469</v>
+        <v>420</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>401</v>
+        <v>469</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>486</v>
+        <v>401</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>677</v>
+        <v>485</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>471</v>
+        <v>677</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>516</v>
+        <v>471</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>491</v>
+        <v>519</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>525</v>
+        <v>493</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>555</v>
+        <v>525</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>488</v>
+        <v>559</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>537</v>
+        <v>488</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>489</v>
+        <v>537</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>676</v>
+        <v>489</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>558</v>
+        <v>679</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>482</v>
+        <v>558</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>546</v>
+        <v>482</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>483</v>
+        <v>548</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>402</v>
+        <v>483</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>509</v>
+        <v>402</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>549</v>
+        <v>509</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>494</v>
+        <v>549</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>555</v>
+        <v>494</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>675</v>
+        <v>555</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>421</v>
+        <v>675</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>550</v>
+        <v>431</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>495</v>
+        <v>551</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>470</v>
+        <v>496</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>526</v>
+        <v>470</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>568</v>
+        <v>527</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>678</v>
+        <v>568</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>499</v>
+        <v>678</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>403</v>
+        <v>500</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>552</v>
+        <v>404</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>528</v>
+        <v>552</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>473</v>
+        <v>529</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>405</v>
+        <v>473</v>
       </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>566</v>
+        <v>406</v>
       </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>373</v>
+        <v>566</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>520</v>
+        <v>373</v>
       </c>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>683</v>
+        <v>518</v>
       </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>517</v>
+        <v>683</v>
       </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>556</v>
+        <v>517</v>
       </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>565</v>
+        <v>556</v>
       </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>536</v>
+        <v>564</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>474</v>
+        <v>536</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>382</v>
+        <v>474</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>408</v>
+        <v>382</v>
       </c>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>530</v>
+        <v>407</v>
       </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>553</v>
+        <v>530</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>383</v>
+        <v>553</v>
       </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>531</v>
+        <v>383</v>
       </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>560</v>
+        <v>531</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>475</v>
+        <v>560</v>
       </c>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>447</v>
+        <v>475</v>
       </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>479</v>
+        <v>449</v>
       </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>512</v>
+        <v>481</v>
       </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>476</v>
+        <v>512</v>
       </c>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>384</v>
+        <v>476</v>
       </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>409</v>
+        <v>385</v>
       </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>502</v>
+        <v>411</v>
       </c>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>386</v>
+        <v>508</v>
       </c>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>450</v>
+        <v>386</v>
       </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>477</v>
+        <v>464</v>
       </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>557</v>
+        <v>477</v>
       </c>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>569</v>
+        <v>557</v>
       </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>532</v>
+        <v>569</v>
       </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>561</v>
+        <v>532</v>
       </c>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>513</v>
+        <v>561</v>
       </c>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>387</v>
+        <v>514</v>
       </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>455</v>
+        <v>387</v>
       </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>432</v>
+        <v>455</v>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>533</v>
+        <v>443</v>
       </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>412</v>
+        <v>533</v>
       </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>478</v>
+        <v>412</v>
       </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>498</v>
+        <v>478</v>
       </c>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>465</v>
+        <v>497</v>
       </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>562</v>
+        <v>515</v>
       </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>388</v>
+        <v>562</v>
       </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>534</v>
+        <v>388</v>
       </c>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>680</v>
+        <v>535</v>
       </c>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>567</v>
+        <v>680</v>
       </c>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>456</v>
+        <v>563</v>
       </c>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>413</v>
+        <v>457</v>
       </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>458</v>
+        <v>414</v>
       </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>501</v>
+        <v>468</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>415</v>
+        <v>501</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="406" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A406" s="1" t="s">
+    <row r="407" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A407" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="B406" s="1" t="s">
+      <c r="B407" s="1" t="s">
         <v>393</v>
-      </c>
-    </row>
-    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A408" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>582</v>
+        <v>622</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>572</v>
+        <v>582</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>602</v>
+        <v>572</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>590</v>
+        <v>602</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>580</v>
+        <v>590</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>621</v>
+        <v>589</v>
       </c>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>591</v>
+        <v>621</v>
       </c>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>573</v>
+        <v>591</v>
       </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>623</v>
+        <v>575</v>
       </c>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>615</v>
+        <v>625</v>
       </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>592</v>
+        <v>616</v>
       </c>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>633</v>
+        <v>596</v>
       </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>597</v>
+        <v>634</v>
       </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>619</v>
+        <v>599</v>
       </c>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>578</v>
+        <v>619</v>
       </c>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>626</v>
+        <v>578</v>
       </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>576</v>
+        <v>627</v>
       </c>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>571</v>
+        <v>576</v>
       </c>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>618</v>
+        <v>571</v>
       </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
-        <v>612</v>
+        <v>618</v>
       </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
-        <v>604</v>
+        <v>620</v>
       </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>581</v>
+        <v>607</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
-        <v>632</v>
+        <v>577</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
-        <v>579</v>
+        <v>632</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
-        <v>670</v>
+        <v>579</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>389</v>
+        <v>670</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
-        <v>574</v>
+        <v>389</v>
       </c>
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
-        <v>629</v>
+        <v>574</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A475" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="478" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A478" s="1" t="s">
+    <row r="479" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A479" s="1" t="s">
         <v>636</v>
       </c>
-      <c r="B478" s="1"/>
-    </row>
-    <row r="480" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A480" t="s">
-        <v>637</v>
-      </c>
+      <c r="B479" s="1"/>
     </row>
     <row r="481" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="482" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="484" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
-        <v>147</v>
+        <v>649</v>
       </c>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
-        <v>650</v>
+        <v>147</v>
       </c>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="498" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="500" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="501" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
-        <v>190</v>
+        <v>656</v>
       </c>
     </row>
     <row r="502" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
-        <v>657</v>
+        <v>190</v>
       </c>
     </row>
     <row r="503" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="504" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="505" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="506" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="507" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="508" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="509" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="510" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="511" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="512" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="513" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="514" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A515" t="s">
         <v>669</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A480:A514">
-    <sortCondition ref="A480:A514"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A481:A515">
+    <sortCondition ref="A481:A515"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated VC commands to work with C3D
</commit_message>
<xml_diff>
--- a/RFLTools Command Reference.xlsx
+++ b/RFLTools Command Reference.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\LISP\GitHub\RFLTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B06A41-2AB9-4F86-B37D-18D72677B755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5CFFEF-CDFF-4B35-8301-EF14B5013BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2760" yWindow="6555" windowWidth="27930" windowHeight="23445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="692">
   <si>
     <t>RFL Tools Command Listing</t>
   </si>
@@ -2098,6 +2098,9 @@
   </si>
   <si>
     <t>Return intersection between a line and a circle</t>
+  </si>
+  <si>
+    <t>RFL:GETVCURVE3P</t>
   </si>
 </sst>
 </file>
@@ -2466,11 +2469,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B518"/>
+  <dimension ref="A1:B519"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
-      <selection activeCell="B308" sqref="B308"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4501,1089 +4502,1094 @@
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>568</v>
+        <v>678</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>678</v>
+        <v>691</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>499</v>
+        <v>568</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>403</v>
+        <v>500</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>552</v>
+        <v>404</v>
       </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>528</v>
+        <v>552</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>473</v>
+        <v>529</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>405</v>
+        <v>473</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>689</v>
-      </c>
-      <c r="B307" t="s">
-        <v>690</v>
+        <v>405</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>406</v>
+        <v>689</v>
+      </c>
+      <c r="B308" t="s">
+        <v>690</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>566</v>
+        <v>406</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>373</v>
+        <v>566</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>520</v>
+        <v>373</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>683</v>
+        <v>518</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>517</v>
+        <v>683</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>556</v>
+        <v>517</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>565</v>
+        <v>556</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>536</v>
+        <v>564</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>474</v>
+        <v>536</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>382</v>
+        <v>474</v>
       </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>408</v>
+        <v>382</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>530</v>
+        <v>407</v>
       </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>553</v>
+        <v>530</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>383</v>
+        <v>553</v>
       </c>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>531</v>
+        <v>383</v>
       </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>560</v>
+        <v>531</v>
       </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>475</v>
+        <v>560</v>
       </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>447</v>
+        <v>475</v>
       </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>479</v>
+        <v>449</v>
       </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>512</v>
+        <v>481</v>
       </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>476</v>
+        <v>512</v>
       </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>384</v>
+        <v>476</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>409</v>
+        <v>385</v>
       </c>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>502</v>
+        <v>411</v>
       </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>386</v>
+        <v>508</v>
       </c>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>450</v>
+        <v>386</v>
       </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>477</v>
+        <v>464</v>
       </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>557</v>
+        <v>477</v>
       </c>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>569</v>
+        <v>557</v>
       </c>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>532</v>
+        <v>569</v>
       </c>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>561</v>
+        <v>532</v>
       </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>513</v>
+        <v>561</v>
       </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>387</v>
+        <v>514</v>
       </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>455</v>
+        <v>387</v>
       </c>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>432</v>
+        <v>455</v>
       </c>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>533</v>
+        <v>443</v>
       </c>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>412</v>
+        <v>533</v>
       </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>478</v>
+        <v>412</v>
       </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>498</v>
+        <v>478</v>
       </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>465</v>
+        <v>497</v>
       </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>562</v>
+        <v>515</v>
       </c>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>388</v>
+        <v>562</v>
       </c>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>534</v>
+        <v>388</v>
       </c>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>680</v>
+        <v>535</v>
       </c>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>567</v>
+        <v>680</v>
       </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>456</v>
+        <v>563</v>
       </c>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>413</v>
+        <v>457</v>
       </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>458</v>
+        <v>414</v>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>501</v>
+        <v>468</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>415</v>
+        <v>501</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A406" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="409" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A409" s="1" t="s">
+    <row r="410" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A410" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="B409" s="1" t="s">
+      <c r="B410" s="1" t="s">
         <v>393</v>
-      </c>
-    </row>
-    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A411" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>582</v>
+        <v>622</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>572</v>
+        <v>582</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>602</v>
+        <v>572</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>590</v>
+        <v>602</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>580</v>
+        <v>590</v>
       </c>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>621</v>
+        <v>589</v>
       </c>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>591</v>
+        <v>621</v>
       </c>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>573</v>
+        <v>591</v>
       </c>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>623</v>
+        <v>575</v>
       </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>615</v>
+        <v>625</v>
       </c>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>592</v>
+        <v>616</v>
       </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>633</v>
+        <v>596</v>
       </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>597</v>
+        <v>634</v>
       </c>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>619</v>
+        <v>599</v>
       </c>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>578</v>
+        <v>619</v>
       </c>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>626</v>
+        <v>578</v>
       </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
-        <v>576</v>
+        <v>627</v>
       </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>571</v>
+        <v>576</v>
       </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>618</v>
+        <v>571</v>
       </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>612</v>
+        <v>618</v>
       </c>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
-        <v>604</v>
+        <v>620</v>
       </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
-        <v>581</v>
+        <v>607</v>
       </c>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>632</v>
+        <v>577</v>
       </c>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
-        <v>579</v>
+        <v>632</v>
       </c>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
-        <v>670</v>
+        <v>579</v>
       </c>
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
-        <v>389</v>
+        <v>670</v>
       </c>
     </row>
     <row r="474" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
-        <v>574</v>
+        <v>389</v>
       </c>
     </row>
     <row r="475" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
-        <v>629</v>
+        <v>574</v>
       </c>
     </row>
     <row r="476" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="477" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="481" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A481" s="1" t="s">
+    <row r="482" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A482" s="1" t="s">
         <v>636</v>
       </c>
-      <c r="B481" s="1"/>
-    </row>
-    <row r="483" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A483" t="s">
-        <v>637</v>
-      </c>
+      <c r="B482" s="1"/>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
-        <v>688</v>
+        <v>648</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
-        <v>649</v>
+        <v>688</v>
       </c>
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
-        <v>147</v>
+        <v>649</v>
       </c>
     </row>
     <row r="498" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
-        <v>650</v>
+        <v>147</v>
       </c>
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="500" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="501" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="502" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="503" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="504" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="505" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
-        <v>190</v>
+        <v>656</v>
       </c>
     </row>
     <row r="506" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
-        <v>657</v>
+        <v>190</v>
       </c>
     </row>
     <row r="507" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="508" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="509" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="510" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="511" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="512" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="513" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="514" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="515" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="516" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="517" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="518" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A519" t="s">
         <v>669</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A483:A518">
-    <sortCondition ref="A483:A518"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A484:A519">
+    <sortCondition ref="A484:A519"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>